<commit_message>
MOZ: Updated tas1 from
</commit_message>
<xml_diff>
--- a/LF/TAS/Mozambique/mz_lf_tas1_2_participant_202011.xlsx
+++ b/LF/TAS/Mozambique/mz_lf_tas1_2_participant_202011.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\LF\TAS\Mozambique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E72ACC7-AA16-49F6-BBB4-5047879C805B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19C9189-F6B9-4E30-98DC-E248243791DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -116,9 +116,6 @@
     <t>end</t>
   </si>
   <si>
-    <t>p_recorderID</t>
-  </si>
-  <si>
     <t>Select your evaluation unit (EU)</t>
   </si>
   <si>
@@ -302,9 +299,6 @@
     <t>p_code_id</t>
   </si>
   <si>
-    <t>concat(${p_cluster_id}, '-', ${p_id_sequence})</t>
-  </si>
-  <si>
     <t>Registre o codigo exclusivo do entrevistadoem cada teste de diagnostico administrado</t>
   </si>
   <si>
@@ -338,10 +332,16 @@
     <t>p_end</t>
   </si>
   <si>
-    <t>2. TAS FL - Inscrição V2</t>
-  </si>
-  <si>
-    <t>mz_lf_tas1_2_participant_202011_v2</t>
+    <t>p_recorder_id</t>
+  </si>
+  <si>
+    <t>concat(${p_cluster_id}, '-', ${p_recorder_id}, '-', ${p_id_sequence})</t>
+  </si>
+  <si>
+    <t>mz_lf_tas1_2_participant_202011_v3</t>
+  </si>
+  <si>
+    <t>2. TAS FL - Inscrição V3</t>
   </si>
 </sst>
 </file>
@@ -872,10 +872,10 @@
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E23" sqref="E22:E23"/>
+      <selection pane="bottomRight" activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
@@ -912,10 +912,10 @@
         <v>16</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>54</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>55</v>
       </c>
       <c r="G1" s="9" t="s">
         <v>6</v>
@@ -927,7 +927,7 @@
         <v>17</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K1" s="9" t="s">
         <v>8</v>
@@ -948,7 +948,7 @@
         <v>13</v>
       </c>
       <c r="Q1" s="34" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="1" customFormat="1" ht="62.7" x14ac:dyDescent="0.55000000000000004">
@@ -956,7 +956,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>28</v>
+        <v>100</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>18</v>
@@ -965,25 +965,25 @@
         <v>19</v>
       </c>
       <c r="E2" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="15" t="s">
         <v>65</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>66</v>
       </c>
       <c r="G2" s="16"/>
       <c r="H2" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J2" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K2" s="16"/>
       <c r="L2" s="16"/>
       <c r="M2" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N2" s="16"/>
       <c r="O2" s="16"/>
@@ -994,14 +994,14 @@
         <v>22</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F3" s="15"/>
       <c r="G3" s="16"/>
@@ -1011,7 +1011,7 @@
       <c r="K3" s="12"/>
       <c r="L3" s="22"/>
       <c r="M3" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N3" s="22"/>
       <c r="O3" s="22"/>
@@ -1022,14 +1022,14 @@
         <v>22</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F4" s="15"/>
       <c r="G4" s="16"/>
@@ -1039,7 +1039,7 @@
       <c r="K4" s="13"/>
       <c r="L4" s="22"/>
       <c r="M4" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N4" s="22"/>
       <c r="O4" s="22"/>
@@ -1050,14 +1050,14 @@
         <v>22</v>
       </c>
       <c r="B5" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="14" t="s">
         <v>30</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>31</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F5" s="15"/>
       <c r="G5" s="16"/>
@@ -1067,7 +1067,7 @@
       <c r="K5" s="13"/>
       <c r="L5" s="22"/>
       <c r="M5" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N5" s="22"/>
       <c r="O5" s="22"/>
@@ -1078,14 +1078,14 @@
         <v>22</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F6" s="15"/>
       <c r="G6" s="16"/>
@@ -1095,7 +1095,7 @@
       <c r="K6" s="13"/>
       <c r="L6" s="22"/>
       <c r="M6" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N6" s="22"/>
       <c r="O6" s="22"/>
@@ -1106,14 +1106,14 @@
         <v>24</v>
       </c>
       <c r="B7" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="20" t="s">
         <v>33</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>34</v>
       </c>
       <c r="D7" s="20"/>
       <c r="E7" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="22"/>
@@ -1123,7 +1123,7 @@
       <c r="K7" s="22"/>
       <c r="L7" s="22"/>
       <c r="M7" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N7" s="22"/>
       <c r="O7" s="22"/>
@@ -1131,17 +1131,17 @@
     </row>
     <row r="8" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="20" t="s">
         <v>35</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>36</v>
       </c>
       <c r="D8" s="20"/>
       <c r="E8" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="22"/>
@@ -1149,11 +1149,11 @@
       <c r="I8" s="20"/>
       <c r="J8" s="25"/>
       <c r="K8" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L8" s="22"/>
       <c r="M8" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N8" s="22"/>
       <c r="O8" s="22"/>
@@ -1164,32 +1164,32 @@
         <v>20</v>
       </c>
       <c r="B9" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>37</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>38</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="13"/>
       <c r="H9" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="I9" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="I9" s="14" t="s">
+      <c r="J9" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="J9" s="15" t="s">
-        <v>81</v>
-      </c>
       <c r="K9" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L9" s="13"/>
       <c r="M9" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N9" s="13"/>
       <c r="O9" s="13"/>
@@ -1200,32 +1200,32 @@
         <v>20</v>
       </c>
       <c r="B10" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>40</v>
       </c>
       <c r="D10" s="20"/>
       <c r="E10" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="16"/>
       <c r="H10" s="23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J10" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L10" s="16"/>
       <c r="M10" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N10" s="16"/>
       <c r="O10" s="16"/>
@@ -1236,30 +1236,30 @@
         <v>20</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>85</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="21" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F11" s="21"/>
       <c r="H11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I11" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="J11" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="J11" s="25" t="s">
-        <v>88</v>
-      </c>
       <c r="K11" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:17" s="1" customFormat="1" ht="47" x14ac:dyDescent="0.55000000000000004">
@@ -1267,44 +1267,44 @@
         <v>22</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="28" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F12" s="28"/>
       <c r="I12" s="8"/>
       <c r="J12" s="25"/>
       <c r="K12" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:17" s="1" customFormat="1" ht="31.35" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="27" t="s">
         <v>41</v>
-      </c>
-      <c r="C13" s="27" t="s">
-        <v>42</v>
       </c>
       <c r="D13" s="27"/>
       <c r="E13" s="28" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F13" s="28"/>
       <c r="G13" s="12"/>
@@ -1312,7 +1312,7 @@
       <c r="I13" s="29"/>
       <c r="J13" s="25"/>
       <c r="K13" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L13" s="12"/>
       <c r="M13" s="13"/>
@@ -1325,14 +1325,14 @@
         <v>25</v>
       </c>
       <c r="B14" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="27" t="s">
         <v>43</v>
-      </c>
-      <c r="C14" s="27" t="s">
-        <v>44</v>
       </c>
       <c r="D14" s="27"/>
       <c r="E14" s="28" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F14" s="28"/>
       <c r="G14" s="12"/>
@@ -1351,7 +1351,7 @@
         <v>26</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C15" s="27"/>
       <c r="D15" s="27"/>
@@ -1373,7 +1373,7 @@
         <v>27</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C16" s="32"/>
       <c r="D16" s="32"/>
@@ -1424,7 +1424,7 @@
         <v>15</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>21</v>
@@ -1435,13 +1435,13 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1449,41 +1449,41 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" t="s">
         <v>61</v>
-      </c>
-      <c r="C3" t="s">
-        <v>96</v>
-      </c>
-      <c r="D3" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1499,13 +1499,13 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="44.109375" customWidth="1"/>
-    <col min="2" max="2" width="19.38671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" customWidth="1"/>
+    <col min="2" max="2" width="38.0546875" customWidth="1"/>
     <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1525,16 +1525,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
         <v>102</v>
-      </c>
-      <c r="B2" t="s">
-        <v>103</v>
       </c>
       <c r="C2">
         <v>20201111</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>